<commit_message>
changement de la représentation du résultat final
</commit_message>
<xml_diff>
--- a/chalal.xlsx
+++ b/chalal.xlsx
@@ -167,9 +167,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +215,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -812,6 +817,81 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,6 +901,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -836,69 +928,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,30 +944,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="16" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1000,6 +1005,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="GBox" noThreeD="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1012,8 +1025,8 @@
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>174172</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>51707</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1064,6 +1077,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>9524</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>180974</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Group Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>38101</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>1333500</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Group Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:noFill/>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1396,12 +1517,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,17 +1547,17 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="76" t="s">
@@ -1465,7 +1586,7 @@
       </c>
       <c r="J3" s="60"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="76" t="s">
         <v>43</v>
       </c>
@@ -1492,7 +1613,7 @@
       </c>
       <c r="J4" s="60"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
         <v>29</v>
       </c>
@@ -1507,10 +1628,10 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
         <v>29</v>
       </c>
@@ -1525,7 +1646,7 @@
         <v>31</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1543,7 +1664,7 @@
         <v>4</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1674,14 +1795,14 @@
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="94"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="119"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="76" t="s">
@@ -1707,22 +1828,22 @@
       <c r="B21" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="128">
-        <v>1</v>
-      </c>
-      <c r="D21" s="127">
+      <c r="C21" s="93">
+        <v>1</v>
+      </c>
+      <c r="D21" s="92" t="b">
         <f>IF(K5=1,7,IF(K5=2,5,IF(K5=3,3,IF(K5=4,1,IF(K5=5,0.3333,IF(K5=6,0.2,IF(K5=7,1/7)))))))</f>
-        <v>7</v>
-      </c>
-      <c r="E21" s="127">
+        <v>0</v>
+      </c>
+      <c r="E21" s="92">
         <f>IF(K6=1,7,IF(K6=2,5,IF(K6=3,3,IF(K6=4,1,IF(K6=5,0.3333,IF(K6=6,0.2,IF(K6=7,1/7)))))))</f>
-        <v>5</v>
-      </c>
-      <c r="F21" s="127">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="92">
         <f>IF(K7=1,7,IF(K7=2,5,IF(K7=3,3,IF(K7=4,1,IF(K7=5,0.3333,IF(K7=6,0.2,IF(K7=7,1/7)))))))</f>
-        <v>3</v>
-      </c>
-      <c r="G21" s="129">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G21" s="94">
         <f>IF(K8=1,7,IF(K8=2,5,IF(K8=3,3,IF(K8=4,1,IF(K8=5,0.3333,IF(K8=6,0.2,IF(K8=7,1/7)))))))</f>
         <v>1</v>
       </c>
@@ -1731,22 +1852,22 @@
       <c r="B22" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="127">
+      <c r="C22" s="92" t="e">
         <f>1/D21</f>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="D22" s="128">
-        <v>1</v>
-      </c>
-      <c r="E22" s="127">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D22" s="93">
+        <v>1</v>
+      </c>
+      <c r="E22" s="92">
         <f>IF(K9=1,7,IF(K9=2,5,IF(K9=3,3,IF(K9=4,1,IF(K9=5,0.3333,IF(K9=6,0.2,IF(K9=7,1/7)))))))</f>
         <v>0.33329999999999999</v>
       </c>
-      <c r="F22" s="127">
+      <c r="F22" s="92">
         <f>IF(K10=1,7,IF(K10=2,5,IF(K10=3,3,IF(K10=4,1,IF(K10=5,0.3333,IF(K10=6,0.2,IF(K10=7,1/7)))))))</f>
         <v>0.2</v>
       </c>
-      <c r="G22" s="129">
+      <c r="G22" s="94">
         <f>IF(K11=1,7,IF(K11=2,5,IF(K11=3,3,IF(K11=4,1,IF(K11=5,0.3333,IF(K11=6,0.2,IF(K11=7,1/7)))))))</f>
         <v>0.14285714285714285</v>
       </c>
@@ -1755,22 +1876,22 @@
       <c r="B23" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="127">
+      <c r="C23" s="92">
         <f>1/E21</f>
-        <v>0.2</v>
-      </c>
-      <c r="D23" s="127">
+        <v>5</v>
+      </c>
+      <c r="D23" s="92">
         <f>1/E22</f>
         <v>3.0003000300030003</v>
       </c>
-      <c r="E23" s="128">
-        <v>1</v>
-      </c>
-      <c r="F23" s="127">
+      <c r="E23" s="93">
+        <v>1</v>
+      </c>
+      <c r="F23" s="92">
         <f>IF(K12=1,7,IF(K12=2,5,IF(K12=3,3,IF(K12=4,1,IF(K12=5,0.3333,IF(K12=6,0.2,IF(K12=7,1/7)))))))</f>
         <v>7</v>
       </c>
-      <c r="G23" s="129">
+      <c r="G23" s="94">
         <f>IF(K13=1,7,IF(K13=2,5,IF(K13=3,3,IF(K13=4,1,IF(K13=5,0.3333,IF(K13=6,0.2,IF(K13=7,1/7)))))))</f>
         <v>7</v>
       </c>
@@ -1779,22 +1900,22 @@
       <c r="B24" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="130">
+      <c r="C24" s="95">
         <f>1/F21</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D24" s="130">
+        <v>7</v>
+      </c>
+      <c r="D24" s="95">
         <f>1/F22</f>
         <v>5</v>
       </c>
-      <c r="E24" s="130">
+      <c r="E24" s="95">
         <f>1/F23</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="F24" s="128">
-        <v>1</v>
-      </c>
-      <c r="G24" s="131">
+      <c r="F24" s="93">
+        <v>1</v>
+      </c>
+      <c r="G24" s="96">
         <f>IF(K14=1,7,IF(K14=2,5,IF(K14=3,3,IF(K14=4,1,IF(K14=5,0.3333,IF(K14=6,0.2,IF(K14=7,1/7)))))))</f>
         <v>7</v>
       </c>
@@ -1803,23 +1924,23 @@
       <c r="B25" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="130">
+      <c r="C25" s="95">
         <f>1/G21</f>
         <v>1</v>
       </c>
-      <c r="D25" s="130">
+      <c r="D25" s="95">
         <f>1/G22</f>
         <v>7</v>
       </c>
-      <c r="E25" s="130">
+      <c r="E25" s="95">
         <f>1/G23</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="F25" s="130">
+      <c r="F25" s="95">
         <f>1/G24</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="G25" s="132">
+      <c r="G25" s="97">
         <v>1</v>
       </c>
     </row>
@@ -1827,37 +1948,37 @@
       <c r="B26" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="133">
+      <c r="C26" s="98" t="e">
         <f>SUM(C21:C25)</f>
-        <v>2.676190476190476</v>
-      </c>
-      <c r="D26" s="133">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D26" s="98">
         <f>SUM(D21:D25)</f>
-        <v>23.000300030003</v>
-      </c>
-      <c r="E26" s="133">
+        <v>16.000300030003</v>
+      </c>
+      <c r="E26" s="98">
         <f>SUM(E21:E25)</f>
-        <v>6.6190142857142868</v>
-      </c>
-      <c r="F26" s="133">
+        <v>1.8190142857142857</v>
+      </c>
+      <c r="F26" s="98">
         <f>SUM(F21:F25)</f>
-        <v>11.342857142857142</v>
-      </c>
-      <c r="G26" s="134">
+        <v>8.485714285714284</v>
+      </c>
+      <c r="G26" s="99">
         <f>SUM(G21:G25)</f>
         <v>16.142857142857142</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="94"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="119"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="76" t="s">
@@ -1883,21 +2004,21 @@
       <c r="B33" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="17" t="e">
         <f t="shared" ref="C33:G37" si="0">C21/C$26</f>
-        <v>0.37366548042704628</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D33" s="17">
         <f t="shared" si="0"/>
-        <v>0.30434385598747715</v>
+        <v>0</v>
       </c>
       <c r="E33" s="17">
         <f t="shared" si="0"/>
-        <v>0.75539948762331888</v>
+        <v>0.10994965876338049</v>
       </c>
       <c r="F33" s="17">
         <f t="shared" si="0"/>
-        <v>0.26448362720403024</v>
+        <v>1.6835016835016838E-2</v>
       </c>
       <c r="G33" s="65">
         <f t="shared" si="0"/>
@@ -1908,21 +2029,21 @@
       <c r="B34" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="17" t="e">
         <f t="shared" si="0"/>
-        <v>5.3380782918149468E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D34" s="17">
         <f t="shared" si="0"/>
-        <v>4.347769371249674E-2</v>
+        <v>6.2498828029777423E-2</v>
       </c>
       <c r="E34" s="17">
         <f t="shared" si="0"/>
-        <v>5.0354929844970434E-2</v>
+        <v>0.18323110632917355</v>
       </c>
       <c r="F34" s="17">
         <f t="shared" si="0"/>
-        <v>1.7632241813602019E-2</v>
+        <v>2.3569023569023576E-2</v>
       </c>
       <c r="G34" s="65">
         <f t="shared" si="0"/>
@@ -1933,21 +2054,21 @@
       <c r="B35" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="17" t="e">
         <f t="shared" si="0"/>
-        <v>7.4733096085409262E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D35" s="17">
         <f t="shared" si="0"/>
-        <v>0.13044612575006523</v>
+        <v>0.18751523561289354</v>
       </c>
       <c r="E35" s="17">
         <f t="shared" si="0"/>
-        <v>0.15107989752466378</v>
+        <v>0.54974829381690238</v>
       </c>
       <c r="F35" s="17">
         <f t="shared" si="0"/>
-        <v>0.61712846347607064</v>
+        <v>0.82491582491582505</v>
       </c>
       <c r="G35" s="65">
         <f t="shared" si="0"/>
@@ -1958,21 +2079,21 @@
       <c r="B36" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="17" t="e">
         <f t="shared" si="0"/>
-        <v>0.12455516014234876</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D36" s="17">
         <f t="shared" si="0"/>
-        <v>0.2173884685624837</v>
+        <v>0.3124941401488871</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" si="0"/>
-        <v>2.1582842503523395E-2</v>
+        <v>7.8535470545271768E-2</v>
       </c>
       <c r="F36" s="17">
         <f t="shared" si="0"/>
-        <v>8.8161209068010088E-2</v>
+        <v>0.11784511784511786</v>
       </c>
       <c r="G36" s="65">
         <f t="shared" si="0"/>
@@ -1983,21 +2104,21 @@
       <c r="B37" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="17" t="e">
         <f t="shared" si="0"/>
-        <v>0.37366548042704628</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D37" s="17">
         <f t="shared" si="0"/>
-        <v>0.30434385598747715</v>
+        <v>0.43749179620844192</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="0"/>
-        <v>2.1582842503523395E-2</v>
+        <v>7.8535470545271768E-2</v>
       </c>
       <c r="F37" s="17">
         <f t="shared" si="0"/>
-        <v>1.2594458438287154E-2</v>
+        <v>1.6835016835016838E-2</v>
       </c>
       <c r="G37" s="65">
         <f t="shared" si="0"/>
@@ -2008,9 +2129,9 @@
       <c r="B38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="25" t="e">
         <f>SUM(C33:C37)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D38" s="25">
         <f>SUM(D33:D37)</f>
@@ -2018,7 +2139,7 @@
       </c>
       <c r="E38" s="25">
         <f>SUM(E33:E37)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="F38" s="25">
         <f>SUM(F33:F37)</f>
@@ -2031,18 +2152,18 @@
     </row>
     <row r="42" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="99"/>
-      <c r="E43" s="95"/>
-      <c r="F43" s="96"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="96"/>
-      <c r="I43" s="96"/>
-      <c r="J43" s="96"/>
-      <c r="K43" s="96"/>
-      <c r="L43" s="97"/>
+      <c r="C43" s="128"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="125"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="125"/>
+      <c r="I43" s="125"/>
+      <c r="J43" s="125"/>
+      <c r="K43" s="125"/>
+      <c r="L43" s="126"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="76" t="s">
@@ -2086,238 +2207,238 @@
       <c r="B45" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="70">
+      <c r="C45" s="70" t="e">
         <f t="shared" ref="C45:C50" si="3">SUM(C33:F33)/4</f>
-        <v>0.42447311281046818</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E45" s="61" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">Communauté </v>
       </c>
-      <c r="F45" s="17">
-        <f t="shared" si="1"/>
-        <v>0.37366548042704628</v>
+      <c r="F45" s="17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G45" s="17">
         <f t="shared" si="1"/>
-        <v>0.30434385598747715</v>
+        <v>0</v>
       </c>
       <c r="H45" s="17">
         <f t="shared" si="1"/>
-        <v>0.75539948762331888</v>
+        <v>0.10994965876338049</v>
       </c>
       <c r="I45" s="17">
         <f t="shared" si="1"/>
-        <v>0.26448362720403024</v>
+        <v>1.6835016835016838E-2</v>
       </c>
       <c r="J45" s="17">
         <f t="shared" si="2"/>
         <v>6.1946902654867256E-2</v>
       </c>
-      <c r="K45" s="89">
+      <c r="K45" s="89" t="e">
         <f>SUM(F45:J45)</f>
-        <v>1.7598393538967401</v>
-      </c>
-      <c r="L45" s="86">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="86" t="e">
         <f>K45/C45</f>
-        <v>4.1459383428192007</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="70">
+      <c r="C46" s="70" t="e">
         <f t="shared" si="3"/>
-        <v>4.1211412072304665E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E46" s="61" t="str">
         <f t="shared" si="1"/>
         <v>Documentation</v>
       </c>
-      <c r="F46" s="17">
-        <f t="shared" si="1"/>
-        <v>5.3380782918149468E-2</v>
+      <c r="F46" s="17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G46" s="17">
         <f t="shared" si="1"/>
-        <v>4.347769371249674E-2</v>
+        <v>6.2498828029777423E-2</v>
       </c>
       <c r="H46" s="17">
         <f t="shared" si="1"/>
-        <v>5.0354929844970434E-2</v>
+        <v>0.18323110632917355</v>
       </c>
       <c r="I46" s="17">
         <f t="shared" si="1"/>
-        <v>1.7632241813602019E-2</v>
+        <v>2.3569023569023576E-2</v>
       </c>
       <c r="J46" s="17">
         <f t="shared" si="2"/>
         <v>8.8495575221238937E-3</v>
       </c>
-      <c r="K46" s="89">
+      <c r="K46" s="89" t="e">
         <f>SUM(F46:J46)</f>
-        <v>0.17369520581134257</v>
-      </c>
-      <c r="L46" s="86">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L46" s="86" t="e">
         <f>K46/C46</f>
-        <v>4.2147356054336971</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="70">
+      <c r="C47" s="70" t="e">
         <f t="shared" si="3"/>
-        <v>0.24334689570905221</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E47" s="61" t="str">
         <f t="shared" si="1"/>
         <v>Niveau d'accessibilité</v>
       </c>
-      <c r="F47" s="17">
-        <f t="shared" si="1"/>
-        <v>7.4733096085409262E-2</v>
+      <c r="F47" s="17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G47" s="17">
         <f t="shared" si="1"/>
-        <v>0.13044612575006523</v>
+        <v>0.18751523561289354</v>
       </c>
       <c r="H47" s="17">
         <f t="shared" si="1"/>
-        <v>0.15107989752466378</v>
+        <v>0.54974829381690238</v>
       </c>
       <c r="I47" s="17">
         <f t="shared" si="1"/>
-        <v>0.61712846347607064</v>
+        <v>0.82491582491582505</v>
       </c>
       <c r="J47" s="17">
         <f t="shared" si="2"/>
         <v>0.4336283185840708</v>
       </c>
-      <c r="K47" s="89">
+      <c r="K47" s="89" t="e">
         <f>SUM(F47:J47)</f>
-        <v>1.4070159014202797</v>
-      </c>
-      <c r="L47" s="86">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="86" t="e">
         <f>K47/C47</f>
-        <v>5.7819348684132006</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="70">
+      <c r="C48" s="70" t="e">
         <f t="shared" si="3"/>
-        <v>0.11292192006909149</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E48" s="61" t="str">
         <f t="shared" si="1"/>
         <v>Sécurité</v>
       </c>
-      <c r="F48" s="17">
-        <f t="shared" si="1"/>
-        <v>0.12455516014234876</v>
+      <c r="F48" s="17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G48" s="17">
         <f t="shared" si="1"/>
-        <v>0.2173884685624837</v>
+        <v>0.3124941401488871</v>
       </c>
       <c r="H48" s="17">
         <f t="shared" si="1"/>
-        <v>2.1582842503523395E-2</v>
+        <v>7.8535470545271768E-2</v>
       </c>
       <c r="I48" s="17">
         <f t="shared" si="1"/>
-        <v>8.8161209068010088E-2</v>
+        <v>0.11784511784511786</v>
       </c>
       <c r="J48" s="17">
         <f t="shared" si="2"/>
         <v>0.4336283185840708</v>
       </c>
-      <c r="K48" s="89">
+      <c r="K48" s="89" t="e">
         <f>SUM(F48:J48)</f>
-        <v>0.88531599886043677</v>
-      </c>
-      <c r="L48" s="86">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L48" s="86" t="e">
         <f>K48/C48</f>
-        <v>7.8400721340794997</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="70">
+      <c r="C49" s="70" t="e">
         <f t="shared" si="3"/>
-        <v>0.17804665933908348</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E49" s="63" t="str">
         <f t="shared" si="1"/>
         <v>Taux d’activité</v>
       </c>
-      <c r="F49" s="26">
-        <f t="shared" si="1"/>
-        <v>0.37366548042704628</v>
+      <c r="F49" s="26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G49" s="26">
         <f t="shared" si="1"/>
-        <v>0.30434385598747715</v>
+        <v>0.43749179620844192</v>
       </c>
       <c r="H49" s="26">
         <f t="shared" si="1"/>
-        <v>2.1582842503523395E-2</v>
+        <v>7.8535470545271768E-2</v>
       </c>
       <c r="I49" s="26">
         <f t="shared" si="1"/>
-        <v>1.2594458438287154E-2</v>
+        <v>1.6835016835016838E-2</v>
       </c>
       <c r="J49" s="26">
         <f t="shared" si="2"/>
         <v>6.1946902654867256E-2</v>
       </c>
-      <c r="K49" s="90">
+      <c r="K49" s="90" t="e">
         <f>SUM(F49:J49)</f>
-        <v>0.77413354001120116</v>
-      </c>
-      <c r="L49" s="87">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L49" s="87" t="e">
         <f>K49/C49</f>
-        <v>4.3479251050528926</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="50" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="71">
+      <c r="C50" s="71" t="e">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="92" t="s">
+      <c r="B54" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="94"/>
+      <c r="C54" s="119"/>
     </row>
     <row r="55" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="56">
+      <c r="C55" s="56" t="e">
         <f>SUM(L45:L49)/5</f>
-        <v>5.2661212111596978</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E55" s="109" t="s">
         <v>41</v>
       </c>
       <c r="F55" s="110"/>
-      <c r="G55" s="113" t="str">
+      <c r="G55" s="113" t="e">
         <f>IF(AND(C57&gt;0,C57&lt;0.1),"Valide","Non Valide")</f>
-        <v>Valide</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H55" s="113"/>
       <c r="I55" s="114"/>
@@ -2326,9 +2447,9 @@
       <c r="B56" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="56">
+      <c r="C56" s="56" t="e">
         <f>(C55-5)/4</f>
-        <v>6.6530302789924445E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E56" s="111"/>
       <c r="F56" s="112"/>
@@ -2340,19 +2461,19 @@
       <c r="B57" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="85">
+      <c r="C57" s="85" t="e">
         <f>C56/1.12</f>
-        <v>5.9402056062432533E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="92" t="s">
+      <c r="B62" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="94"/>
+      <c r="C62" s="118"/>
+      <c r="D62" s="118"/>
+      <c r="E62" s="119"/>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="76" t="s">
@@ -2452,18 +2573,18 @@
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="59"/>
       <c r="C74" s="47"/>
-      <c r="D74" s="117" t="s">
+      <c r="D74" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="117"/>
-      <c r="F74" s="118" t="s">
+      <c r="E74" s="120"/>
+      <c r="F74" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="G74" s="118"/>
-      <c r="H74" s="119" t="s">
+      <c r="G74" s="121"/>
+      <c r="H74" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="I74" s="120"/>
+      <c r="I74" s="123"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="55" t="s">
@@ -2495,165 +2616,165 @@
       <c r="B76" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C76" s="52">
+      <c r="C76" s="52" t="e">
         <f>C45</f>
-        <v>0.42447311281046818</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D76" s="49">
         <f>C64</f>
         <v>4</v>
       </c>
-      <c r="E76" s="49">
+      <c r="E76" s="49" t="e">
         <f>D76*C76</f>
-        <v>1.6978924512418727</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F76" s="50">
         <f>D64</f>
         <v>2</v>
       </c>
-      <c r="G76" s="50">
+      <c r="G76" s="50" t="e">
         <f>C76*F76</f>
-        <v>0.84894622562093636</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H76" s="51">
         <f>E64</f>
         <v>0</v>
       </c>
-      <c r="I76" s="56">
+      <c r="I76" s="56" t="e">
         <f>C76*H76</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="52">
+      <c r="C77" s="52" t="e">
         <f>C46</f>
-        <v>4.1211412072304665E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D77" s="49">
         <f>C65</f>
         <v>4</v>
       </c>
-      <c r="E77" s="49">
+      <c r="E77" s="49" t="e">
         <f t="shared" ref="E77:E79" si="4">D77*C77</f>
-        <v>0.16484564828921866</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F77" s="50">
         <f>D65</f>
         <v>3</v>
       </c>
-      <c r="G77" s="50">
+      <c r="G77" s="50" t="e">
         <f t="shared" ref="G77:G79" si="5">C77*F77</f>
-        <v>0.123634236216914</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H77" s="51">
         <f>E65</f>
         <v>3</v>
       </c>
-      <c r="I77" s="56">
+      <c r="I77" s="56" t="e">
         <f t="shared" ref="I77:I79" si="6">C77*H77</f>
-        <v>0.123634236216914</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="52">
+      <c r="C78" s="52" t="e">
         <f>C47</f>
-        <v>0.24334689570905221</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D78" s="49">
         <f>C66</f>
         <v>4</v>
       </c>
-      <c r="E78" s="49">
+      <c r="E78" s="49" t="e">
         <f t="shared" si="4"/>
-        <v>0.97338758283620885</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F78" s="50">
         <f>D66</f>
         <v>1</v>
       </c>
-      <c r="G78" s="50">
+      <c r="G78" s="50" t="e">
         <f t="shared" si="5"/>
-        <v>0.24334689570905221</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H78" s="51">
         <f>E66</f>
         <v>4</v>
       </c>
-      <c r="I78" s="56">
+      <c r="I78" s="56" t="e">
         <f t="shared" si="6"/>
-        <v>0.97338758283620885</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C79" s="52">
+      <c r="C79" s="52" t="e">
         <f>C48</f>
-        <v>0.11292192006909149</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D79" s="49">
         <f>C67</f>
         <v>0</v>
       </c>
-      <c r="E79" s="49">
+      <c r="E79" s="49" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F79" s="50">
         <f>D67</f>
         <v>1</v>
       </c>
-      <c r="G79" s="50">
+      <c r="G79" s="50" t="e">
         <f t="shared" si="5"/>
-        <v>0.11292192006909149</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H79" s="51">
         <f>E67</f>
         <v>1</v>
       </c>
-      <c r="I79" s="56">
+      <c r="I79" s="56" t="e">
         <f t="shared" si="6"/>
-        <v>0.11292192006909149</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="80" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="81">
+      <c r="C80" s="81" t="e">
         <f>C49</f>
-        <v>0.17804665933908348</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D80" s="82">
         <f>C68</f>
         <v>4</v>
       </c>
-      <c r="E80" s="82">
+      <c r="E80" s="82" t="e">
         <f t="shared" ref="E80" si="7">D80*C80</f>
-        <v>0.71218663735633392</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F80" s="83">
         <f>D68</f>
         <v>3</v>
       </c>
-      <c r="G80" s="83">
+      <c r="G80" s="83" t="e">
         <f t="shared" ref="G80" si="8">C80*F80</f>
-        <v>0.53413997801725044</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H80" s="84">
         <f>E68</f>
         <v>3</v>
       </c>
-      <c r="I80" s="85">
+      <c r="I80" s="85" t="e">
         <f t="shared" ref="I80" si="9">C80*H80</f>
-        <v>0.53413997801725044</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -2698,17 +2819,17 @@
       <c r="B87" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="65">
+      <c r="C87" s="65" t="e">
         <f>SUM(E76:E80)</f>
-        <v>3.5483123197236344</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="F87" s="102" t="str">
+      <c r="F87" s="102" t="e">
         <f>IF(C87&gt;CET88*(C87&gt;C89),B87,IF(C88&gt;C89,B88,B89))</f>
-        <v>pentaho</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G87" s="103"/>
     </row>
@@ -2716,9 +2837,9 @@
       <c r="B88" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C88" s="65">
+      <c r="C88" s="65" t="e">
         <f>SUM(G76:G80)</f>
-        <v>1.8629892556332444</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E88" s="101"/>
       <c r="F88" s="104"/>
@@ -2728,13 +2849,19 @@
       <c r="B89" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="74">
+      <c r="C89" s="74" t="e">
         <f>SUM(I76:I80)</f>
-        <v>1.7440837171394648</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E43:L43"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B43:C43"/>
     <mergeCell ref="E87:E88"/>
     <mergeCell ref="F87:G88"/>
     <mergeCell ref="B73:I73"/>
@@ -2744,12 +2871,6 @@
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="F74:G74"/>
     <mergeCell ref="H74:I74"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="E43:L43"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <conditionalFormatting sqref="G55:I56">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -2768,6 +2889,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Group Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId5" name="Group Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>1333500</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -2800,17 +2972,17 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="94"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -3013,13 +3185,13 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="94"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="119"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="31" t="s">
@@ -3129,13 +3301,13 @@
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="94"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="119"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
@@ -3321,12 +3493,12 @@
     </row>
     <row r="46" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="92" t="s">
+      <c r="B47" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="94"/>
+      <c r="C47" s="118"/>
+      <c r="D47" s="118"/>
+      <c r="E47" s="119"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="31" t="s">
@@ -3402,18 +3574,18 @@
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="53"/>
       <c r="C57" s="54"/>
-      <c r="D57" s="125" t="s">
+      <c r="D57" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="125"/>
-      <c r="F57" s="126" t="s">
-        <v>1</v>
-      </c>
-      <c r="G57" s="126"/>
-      <c r="H57" s="122" t="s">
+      <c r="E57" s="133"/>
+      <c r="F57" s="134" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="134"/>
+      <c r="H57" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="I57" s="123"/>
+      <c r="I57" s="131"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="55" t="s">
@@ -3562,21 +3734,21 @@
         <v>18</v>
       </c>
       <c r="C63" s="58"/>
-      <c r="D63" s="121">
+      <c r="D63" s="129">
         <f>SUM(E59:E62)</f>
         <v>2.3548140709955541</v>
       </c>
-      <c r="E63" s="121"/>
-      <c r="F63" s="121">
+      <c r="E63" s="129"/>
+      <c r="F63" s="129">
         <f t="shared" ref="F63" si="8">SUM(F59:F62)</f>
         <v>8</v>
       </c>
-      <c r="G63" s="121"/>
-      <c r="H63" s="121">
+      <c r="G63" s="129"/>
+      <c r="H63" s="129">
         <f t="shared" ref="H63" si="9">SUM(H59:H62)</f>
         <v>7</v>
       </c>
-      <c r="I63" s="124"/>
+      <c r="I63" s="132"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>

</xml_diff>